<commit_message>
Updated the BeforeAndAfterClass.java file
</commit_message>
<xml_diff>
--- a/Automata/resources/DataSheet.xlsx
+++ b/Automata/resources/DataSheet.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18">
   <si>
     <t>testOne</t>
   </si>
@@ -65,6 +65,12 @@
   </si>
   <si>
     <t>Martian Manhunter</t>
+  </si>
+  <si>
+    <t>Robin</t>
+  </si>
+  <si>
+    <t>Joker</t>
   </si>
 </sst>
 </file>
@@ -282,163 +288,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -578,124 +584,124 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1034,14 +1040,15 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="$A1:$XFD1048576"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="8.88888888888889" style="1"/>
     <col min="2" max="2" width="25.2222222222222" style="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88888888888889" style="1"/>
+    <col min="3" max="3" width="10" style="1" customWidth="1"/>
+    <col min="4" max="4" width="8.88888888888889" style="1"/>
     <col min="5" max="5" width="25.2222222222222" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.6666666666667" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.5555555555556" style="1" customWidth="1"/>
@@ -1166,7 +1173,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:G5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -1234,7 +1241,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -1257,7 +1264,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>6</v>

</xml_diff>